<commit_message>
FEATURE: V12 Multi-school management + Board tracking + Field priority guide
- V12 Migration: Added school_name, board, academic_year columns to students table
- Updated Student entity with 3 new fields + getters/setters
- Updated StudentUploadDto with school/board/academic year fields
- Updated UploadController field mapping (setDtoField + confirmUpload)
- Created FIELD_PRIORITY_GUIDE.md: Comprehensive priority documentation (P0-P3, Optional)
- Updated sample-student-template.csv: Added School Name, Board, Academic Year columns
- Updated sample-student-template.xlsx: Regenerated with new columns
- Multi-school examples: Ryan International, Cambridge HS, St Lawrence HS, DPS, Modern HS, Cathedral, DAV
- Board diversity: CBSE (8 students), ICSE (7 students)
- All 15 students now have complete school/board context for management group scenarios
</commit_message>
<xml_diff>
--- a/sample-student-template.xlsx
+++ b/sample-student-template.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X16"/>
+  <dimension ref="A1:AA16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,29 +436,32 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="12" customWidth="1" min="1" max="1"/>
-    <col width="15" customWidth="1" min="2" max="2"/>
-    <col width="15" customWidth="1" min="3" max="3"/>
-    <col width="8" customWidth="1" min="4" max="4"/>
-    <col width="7" customWidth="1" min="5" max="5"/>
-    <col width="10" customWidth="1" min="6" max="6"/>
-    <col width="14" customWidth="1" min="7" max="7"/>
-    <col width="15" customWidth="1" min="8" max="8"/>
-    <col width="16" customWidth="1" min="9" max="9"/>
-    <col width="16" customWidth="1" min="10" max="10"/>
-    <col width="16" customWidth="1" min="11" max="11"/>
-    <col width="10" customWidth="1" min="12" max="12"/>
-    <col width="30" customWidth="1" min="13" max="13"/>
-    <col width="17" customWidth="1" min="14" max="14"/>
-    <col width="16" customWidth="1" min="15" max="15"/>
-    <col width="15" customWidth="1" min="16" max="16"/>
-    <col width="14" customWidth="1" min="17" max="17"/>
+    <col width="32" customWidth="1" min="2" max="2"/>
+    <col width="7" customWidth="1" min="3" max="3"/>
+    <col width="15" customWidth="1" min="4" max="4"/>
+    <col width="15" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="8" customWidth="1" min="7" max="7"/>
+    <col width="7" customWidth="1" min="8" max="8"/>
+    <col width="10" customWidth="1" min="9" max="9"/>
+    <col width="14" customWidth="1" min="10" max="10"/>
+    <col width="15" customWidth="1" min="11" max="11"/>
+    <col width="16" customWidth="1" min="12" max="12"/>
+    <col width="16" customWidth="1" min="13" max="13"/>
+    <col width="16" customWidth="1" min="14" max="14"/>
+    <col width="10" customWidth="1" min="15" max="15"/>
+    <col width="30" customWidth="1" min="16" max="16"/>
+    <col width="17" customWidth="1" min="17" max="17"/>
     <col width="16" customWidth="1" min="18" max="18"/>
-    <col width="13" customWidth="1" min="19" max="19"/>
-    <col width="12" customWidth="1" min="20" max="20"/>
-    <col width="15" customWidth="1" min="21" max="21"/>
-    <col width="18" customWidth="1" min="22" max="22"/>
-    <col width="19" customWidth="1" min="23" max="23"/>
-    <col width="10" customWidth="1" min="24" max="24"/>
+    <col width="15" customWidth="1" min="19" max="19"/>
+    <col width="14" customWidth="1" min="20" max="20"/>
+    <col width="16" customWidth="1" min="21" max="21"/>
+    <col width="13" customWidth="1" min="22" max="22"/>
+    <col width="12" customWidth="1" min="23" max="23"/>
+    <col width="15" customWidth="1" min="24" max="24"/>
+    <col width="18" customWidth="1" min="25" max="25"/>
+    <col width="19" customWidth="1" min="26" max="26"/>
+    <col width="10" customWidth="1" min="27" max="27"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -469,115 +472,130 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>School Name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Board</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Academic Year</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>Full Name</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Date of Birth</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Gender</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Class</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Division</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Sub-Division</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Father Name</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Father Contact</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Mother Name</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Mother Contact</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Category</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Address</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Admission Class</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Admission Date</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Enrollment No</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>APAAR ID</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>Aadhaar Number</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>Blood Group</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>Fee Status</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>Guardian Name</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>Guardian Contact</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>Guardian Relation</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>Language</t>
         </is>
@@ -591,102 +609,117 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>Ryan International High School</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>CBSE</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2024-2025</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
           <t>Rajesh Kumar</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>15/05/2010</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>General</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>Suresh Kumar</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="L2" t="inlineStr">
         <is>
           <t>9876543210</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="M2" t="inlineStr">
         <is>
           <t>Priya Kumar</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="N2" t="inlineStr">
         <is>
           <t>9876543211</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="O2" t="inlineStr">
         <is>
           <t>General</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
+      <c r="P2" t="inlineStr">
         <is>
           <t>123 MG Road Mumbai</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
+      <c r="Q2" t="inlineStr">
         <is>
           <t>9</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr">
+      <c r="R2" t="inlineStr">
         <is>
           <t>01/04/2023</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr">
+      <c r="S2" t="inlineStr">
         <is>
           <t>EN2023001</t>
         </is>
       </c>
-      <c r="Q2" t="inlineStr">
+      <c r="T2" t="inlineStr">
         <is>
           <t>APR123456789</t>
         </is>
       </c>
-      <c r="R2" t="inlineStr">
+      <c r="U2" t="inlineStr">
         <is>
           <t>123456789012</t>
         </is>
       </c>
-      <c r="S2" t="inlineStr">
+      <c r="V2" t="inlineStr">
         <is>
           <t>O+</t>
         </is>
       </c>
-      <c r="T2" t="inlineStr">
+      <c r="W2" t="inlineStr">
         <is>
           <t>Paid</t>
         </is>
       </c>
-      <c r="U2" t="inlineStr"/>
-      <c r="V2" t="inlineStr"/>
-      <c r="W2" t="inlineStr">
+      <c r="X2" t="inlineStr"/>
+      <c r="Y2" t="inlineStr"/>
+      <c r="Z2" t="inlineStr">
         <is>
           <t>English</t>
         </is>
@@ -700,102 +733,117 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>Ryan International High School</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>CBSE</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2024-2025</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
           <t>Priya Sharma</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>22/08/2010</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>Female</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>General</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="J3" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="K3" t="inlineStr">
         <is>
           <t>Amit Sharma</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="L3" t="inlineStr">
         <is>
           <t>9876543212</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="M3" t="inlineStr">
         <is>
           <t>Neha Sharma</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="N3" t="inlineStr">
         <is>
           <t>9876543213</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr">
+      <c r="O3" t="inlineStr">
         <is>
           <t>OBC</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
+      <c r="P3" t="inlineStr">
         <is>
           <t>456 Park Street Kolkata</t>
         </is>
       </c>
-      <c r="N3" t="inlineStr">
+      <c r="Q3" t="inlineStr">
         <is>
           <t>9</t>
         </is>
       </c>
-      <c r="O3" t="inlineStr">
+      <c r="R3" t="inlineStr">
         <is>
           <t>01/04/2023</t>
         </is>
       </c>
-      <c r="P3" t="inlineStr">
+      <c r="S3" t="inlineStr">
         <is>
           <t>EN2023002</t>
         </is>
       </c>
-      <c r="Q3" t="inlineStr">
+      <c r="T3" t="inlineStr">
         <is>
           <t>APR987654321</t>
         </is>
       </c>
-      <c r="R3" t="inlineStr">
+      <c r="U3" t="inlineStr">
         <is>
           <t>234567890123</t>
         </is>
       </c>
-      <c r="S3" t="inlineStr">
+      <c r="V3" t="inlineStr">
         <is>
           <t>A+</t>
         </is>
       </c>
-      <c r="T3" t="inlineStr">
+      <c r="W3" t="inlineStr">
         <is>
           <t>Pending</t>
         </is>
       </c>
-      <c r="U3" t="inlineStr"/>
-      <c r="V3" t="inlineStr"/>
-      <c r="W3" t="inlineStr">
+      <c r="X3" t="inlineStr"/>
+      <c r="Y3" t="inlineStr"/>
+      <c r="Z3" t="inlineStr">
         <is>
           <t>Hindi</t>
         </is>
@@ -809,98 +857,113 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>Cambridge High School</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>ICSE</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2024-2025</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
           <t>Mohammed Ali</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>10/03/2010</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="I4" t="inlineStr">
         <is>
           <t>General</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="J4" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="K4" t="inlineStr">
         <is>
           <t>Imran Ali</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
+      <c r="L4" t="inlineStr">
         <is>
           <t>9876543214</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
+      <c r="M4" t="inlineStr">
         <is>
           <t>Fatima Ali</t>
         </is>
       </c>
-      <c r="K4" t="inlineStr">
+      <c r="N4" t="inlineStr">
         <is>
           <t>9876543215</t>
         </is>
       </c>
-      <c r="L4" t="inlineStr">
+      <c r="O4" t="inlineStr">
         <is>
           <t>General</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr">
+      <c r="P4" t="inlineStr">
         <is>
           <t>789 Anna Salai Chennai</t>
         </is>
       </c>
-      <c r="N4" t="inlineStr">
+      <c r="Q4" t="inlineStr">
         <is>
           <t>9</t>
         </is>
       </c>
-      <c r="O4" t="inlineStr">
+      <c r="R4" t="inlineStr">
         <is>
           <t>01/04/2023</t>
         </is>
       </c>
-      <c r="P4" t="inlineStr">
+      <c r="S4" t="inlineStr">
         <is>
           <t>EN2023003</t>
         </is>
       </c>
-      <c r="Q4" t="inlineStr"/>
-      <c r="R4" t="inlineStr">
+      <c r="T4" t="inlineStr"/>
+      <c r="U4" t="inlineStr">
         <is>
           <t>345678901234</t>
         </is>
       </c>
-      <c r="S4" t="inlineStr">
+      <c r="V4" t="inlineStr">
         <is>
           <t>B+</t>
         </is>
       </c>
-      <c r="T4" t="inlineStr">
+      <c r="W4" t="inlineStr">
         <is>
           <t>Paid</t>
         </is>
       </c>
-      <c r="U4" t="inlineStr"/>
-      <c r="V4" t="inlineStr"/>
-      <c r="W4" t="inlineStr">
+      <c r="X4" t="inlineStr"/>
+      <c r="Y4" t="inlineStr"/>
+      <c r="Z4" t="inlineStr">
         <is>
           <t>English</t>
         </is>
@@ -914,102 +977,117 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>Cambridge High School</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>ICSE</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2024-2025</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
           <t>Ananya Reddy</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>05/11/2010</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>Female</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="H5" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="I5" t="inlineStr">
         <is>
           <t>General</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="J5" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="K5" t="inlineStr">
         <is>
           <t>Venkat Reddy</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
+      <c r="L5" t="inlineStr">
         <is>
           <t>9876543216</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
+      <c r="M5" t="inlineStr">
         <is>
           <t>Lakshmi Reddy</t>
         </is>
       </c>
-      <c r="K5" t="inlineStr">
+      <c r="N5" t="inlineStr">
         <is>
           <t>9876543217</t>
         </is>
       </c>
-      <c r="L5" t="inlineStr">
+      <c r="O5" t="inlineStr">
         <is>
           <t>General</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr">
+      <c r="P5" t="inlineStr">
         <is>
           <t>321 Brigade Road Bangalore</t>
         </is>
       </c>
-      <c r="N5" t="inlineStr">
+      <c r="Q5" t="inlineStr">
         <is>
           <t>9</t>
         </is>
       </c>
-      <c r="O5" t="inlineStr">
+      <c r="R5" t="inlineStr">
         <is>
           <t>01/04/2023</t>
         </is>
       </c>
-      <c r="P5" t="inlineStr">
+      <c r="S5" t="inlineStr">
         <is>
           <t>EN2023004</t>
         </is>
       </c>
-      <c r="Q5" t="inlineStr">
+      <c r="T5" t="inlineStr">
         <is>
           <t>APR456789123</t>
         </is>
       </c>
-      <c r="R5" t="inlineStr">
+      <c r="U5" t="inlineStr">
         <is>
           <t>456789012345</t>
         </is>
       </c>
-      <c r="S5" t="inlineStr">
+      <c r="V5" t="inlineStr">
         <is>
           <t>AB+</t>
         </is>
       </c>
-      <c r="T5" t="inlineStr">
+      <c r="W5" t="inlineStr">
         <is>
           <t>Paid</t>
         </is>
       </c>
-      <c r="U5" t="inlineStr"/>
-      <c r="V5" t="inlineStr"/>
-      <c r="W5" t="inlineStr">
+      <c r="X5" t="inlineStr"/>
+      <c r="Y5" t="inlineStr"/>
+      <c r="Z5" t="inlineStr">
         <is>
           <t>Telugu</t>
         </is>
@@ -1023,102 +1101,117 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>St Lawrence High School</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>CBSE</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2024-2025</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
           <t>Arjun Patel</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>18/06/2009</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="G6" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="H6" t="inlineStr">
         <is>
           <t>11</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="I6" t="inlineStr">
         <is>
           <t>Science</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="J6" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
+      <c r="K6" t="inlineStr">
         <is>
           <t>Kiran Patel</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
+      <c r="L6" t="inlineStr">
         <is>
           <t>9876543218</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr">
+      <c r="M6" t="inlineStr">
         <is>
           <t>Meera Patel</t>
         </is>
       </c>
-      <c r="K6" t="inlineStr">
+      <c r="N6" t="inlineStr">
         <is>
           <t>9876543219</t>
         </is>
       </c>
-      <c r="L6" t="inlineStr">
+      <c r="O6" t="inlineStr">
         <is>
           <t>General</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr">
+      <c r="P6" t="inlineStr">
         <is>
           <t>654 Law Garden Ahmedabad</t>
         </is>
       </c>
-      <c r="N6" t="inlineStr">
+      <c r="Q6" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
-      <c r="O6" t="inlineStr">
+      <c r="R6" t="inlineStr">
         <is>
           <t>01/04/2022</t>
         </is>
       </c>
-      <c r="P6" t="inlineStr">
+      <c r="S6" t="inlineStr">
         <is>
           <t>EN2022001</t>
         </is>
       </c>
-      <c r="Q6" t="inlineStr">
+      <c r="T6" t="inlineStr">
         <is>
           <t>APR789123456</t>
         </is>
       </c>
-      <c r="R6" t="inlineStr">
+      <c r="U6" t="inlineStr">
         <is>
           <t>567890123456</t>
         </is>
       </c>
-      <c r="S6" t="inlineStr">
+      <c r="V6" t="inlineStr">
         <is>
           <t>O-</t>
         </is>
       </c>
-      <c r="T6" t="inlineStr">
+      <c r="W6" t="inlineStr">
         <is>
           <t>Paid</t>
         </is>
       </c>
-      <c r="U6" t="inlineStr"/>
-      <c r="V6" t="inlineStr"/>
-      <c r="W6" t="inlineStr">
+      <c r="X6" t="inlineStr"/>
+      <c r="Y6" t="inlineStr"/>
+      <c r="Z6" t="inlineStr">
         <is>
           <t>Gujarati</t>
         </is>
@@ -1132,98 +1225,113 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>St Lawrence High School</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>CBSE</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2024-2025</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
           <t>Divya Nair</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>25/09/2009</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="G7" t="inlineStr">
         <is>
           <t>Female</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="H7" t="inlineStr">
         <is>
           <t>11</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="I7" t="inlineStr">
         <is>
           <t>Science</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="J7" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="K7" t="inlineStr">
         <is>
           <t>Sunil Nair</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr">
+      <c r="L7" t="inlineStr">
         <is>
           <t>9876543220</t>
         </is>
       </c>
-      <c r="J7" t="inlineStr">
+      <c r="M7" t="inlineStr">
         <is>
           <t>Asha Nair</t>
         </is>
       </c>
-      <c r="K7" t="inlineStr">
+      <c r="N7" t="inlineStr">
         <is>
           <t>9876543221</t>
         </is>
       </c>
-      <c r="L7" t="inlineStr">
+      <c r="O7" t="inlineStr">
         <is>
           <t>SC</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr">
+      <c r="P7" t="inlineStr">
         <is>
           <t>987 Marine Drive Kochi</t>
         </is>
       </c>
-      <c r="N7" t="inlineStr">
+      <c r="Q7" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
-      <c r="O7" t="inlineStr">
+      <c r="R7" t="inlineStr">
         <is>
           <t>01/04/2022</t>
         </is>
       </c>
-      <c r="P7" t="inlineStr">
+      <c r="S7" t="inlineStr">
         <is>
           <t>EN2022002</t>
         </is>
       </c>
-      <c r="Q7" t="inlineStr"/>
-      <c r="R7" t="inlineStr">
+      <c r="T7" t="inlineStr"/>
+      <c r="U7" t="inlineStr">
         <is>
           <t>678901234567</t>
         </is>
       </c>
-      <c r="S7" t="inlineStr">
+      <c r="V7" t="inlineStr">
         <is>
           <t>A-</t>
         </is>
       </c>
-      <c r="T7" t="inlineStr">
+      <c r="W7" t="inlineStr">
         <is>
           <t>Waived</t>
         </is>
       </c>
-      <c r="U7" t="inlineStr"/>
-      <c r="V7" t="inlineStr"/>
-      <c r="W7" t="inlineStr">
+      <c r="X7" t="inlineStr"/>
+      <c r="Y7" t="inlineStr"/>
+      <c r="Z7" t="inlineStr">
         <is>
           <t>Malayalam</t>
         </is>
@@ -1237,102 +1345,117 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
+          <t>DAV Public School</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>CBSE</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2024-2025</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
           <t>Kabir Singh</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>30/01/2009</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="G8" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="H8" t="inlineStr">
         <is>
           <t>11</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="I8" t="inlineStr">
         <is>
           <t>Commerce</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
+      <c r="J8" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
+      <c r="K8" t="inlineStr">
         <is>
           <t>Rajesh Singh</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr">
+      <c r="L8" t="inlineStr">
         <is>
           <t>9876543222</t>
         </is>
       </c>
-      <c r="J8" t="inlineStr">
+      <c r="M8" t="inlineStr">
         <is>
           <t>Anjali Singh</t>
         </is>
       </c>
-      <c r="K8" t="inlineStr">
+      <c r="N8" t="inlineStr">
         <is>
           <t>9876543223</t>
         </is>
       </c>
-      <c r="L8" t="inlineStr">
+      <c r="O8" t="inlineStr">
         <is>
           <t>General</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr">
+      <c r="P8" t="inlineStr">
         <is>
           <t>147 Connaught Place Delhi</t>
         </is>
       </c>
-      <c r="N8" t="inlineStr">
+      <c r="Q8" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
-      <c r="O8" t="inlineStr">
+      <c r="R8" t="inlineStr">
         <is>
           <t>01/04/2022</t>
         </is>
       </c>
-      <c r="P8" t="inlineStr">
+      <c r="S8" t="inlineStr">
         <is>
           <t>EN2022003</t>
         </is>
       </c>
-      <c r="Q8" t="inlineStr">
+      <c r="T8" t="inlineStr">
         <is>
           <t>APR321654987</t>
         </is>
       </c>
-      <c r="R8" t="inlineStr">
+      <c r="U8" t="inlineStr">
         <is>
           <t>789012345678</t>
         </is>
       </c>
-      <c r="S8" t="inlineStr">
+      <c r="V8" t="inlineStr">
         <is>
           <t>B-</t>
         </is>
       </c>
-      <c r="T8" t="inlineStr">
+      <c r="W8" t="inlineStr">
         <is>
           <t>Paid</t>
         </is>
       </c>
-      <c r="U8" t="inlineStr"/>
-      <c r="V8" t="inlineStr"/>
-      <c r="W8" t="inlineStr">
+      <c r="X8" t="inlineStr"/>
+      <c r="Y8" t="inlineStr"/>
+      <c r="Z8" t="inlineStr">
         <is>
           <t>Hindi</t>
         </is>
@@ -1346,102 +1469,117 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
+          <t>Cathedral School</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>ICSE</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2024-2025</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
           <t>Zara Khan</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="F9" t="inlineStr">
         <is>
           <t>12/12/2009</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="G9" t="inlineStr">
         <is>
           <t>Female</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="H9" t="inlineStr">
         <is>
           <t>11</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="I9" t="inlineStr">
         <is>
           <t>Science</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
+      <c r="J9" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
+      <c r="K9" t="inlineStr">
         <is>
           <t>Salman Khan</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr">
+      <c r="L9" t="inlineStr">
         <is>
           <t>9876543224</t>
         </is>
       </c>
-      <c r="J9" t="inlineStr">
+      <c r="M9" t="inlineStr">
         <is>
           <t>Ayesha Khan</t>
         </is>
       </c>
-      <c r="K9" t="inlineStr">
+      <c r="N9" t="inlineStr">
         <is>
           <t>9876543225</t>
         </is>
       </c>
-      <c r="L9" t="inlineStr">
+      <c r="O9" t="inlineStr">
         <is>
           <t>General</t>
         </is>
       </c>
-      <c r="M9" t="inlineStr">
+      <c r="P9" t="inlineStr">
         <is>
           <t>258 Park Street Hyderabad</t>
         </is>
       </c>
-      <c r="N9" t="inlineStr">
+      <c r="Q9" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
-      <c r="O9" t="inlineStr">
+      <c r="R9" t="inlineStr">
         <is>
           <t>01/04/2022</t>
         </is>
       </c>
-      <c r="P9" t="inlineStr">
+      <c r="S9" t="inlineStr">
         <is>
           <t>EN2022004</t>
         </is>
       </c>
-      <c r="Q9" t="inlineStr">
+      <c r="T9" t="inlineStr">
         <is>
           <t>APR654987321</t>
         </is>
       </c>
-      <c r="R9" t="inlineStr">
+      <c r="U9" t="inlineStr">
         <is>
           <t>890123456789</t>
         </is>
       </c>
-      <c r="S9" t="inlineStr">
+      <c r="V9" t="inlineStr">
         <is>
           <t>AB-</t>
         </is>
       </c>
-      <c r="T9" t="inlineStr">
+      <c r="W9" t="inlineStr">
         <is>
           <t>Paid</t>
         </is>
       </c>
-      <c r="U9" t="inlineStr"/>
-      <c r="V9" t="inlineStr"/>
-      <c r="W9" t="inlineStr">
+      <c r="X9" t="inlineStr"/>
+      <c r="Y9" t="inlineStr"/>
+      <c r="Z9" t="inlineStr">
         <is>
           <t>Urdu</t>
         </is>
@@ -1455,102 +1593,117 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
+          <t>Delhi Public School</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>CBSE</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>2024-2025</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
           <t>Advait Joshi</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>08/04/2011</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="G10" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="H10" t="inlineStr">
         <is>
           <t>9</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="I10" t="inlineStr">
         <is>
           <t>General</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
+      <c r="J10" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
+      <c r="K10" t="inlineStr">
         <is>
           <t>Prakash Joshi</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr">
+      <c r="L10" t="inlineStr">
         <is>
           <t>9876543226</t>
         </is>
       </c>
-      <c r="J10" t="inlineStr">
+      <c r="M10" t="inlineStr">
         <is>
           <t>Swati Joshi</t>
         </is>
       </c>
-      <c r="K10" t="inlineStr">
+      <c r="N10" t="inlineStr">
         <is>
           <t>9876543227</t>
         </is>
       </c>
-      <c r="L10" t="inlineStr">
+      <c r="O10" t="inlineStr">
         <is>
           <t>General</t>
         </is>
       </c>
-      <c r="M10" t="inlineStr">
+      <c r="P10" t="inlineStr">
         <is>
           <t>369 FC Road Pune</t>
         </is>
       </c>
-      <c r="N10" t="inlineStr">
+      <c r="Q10" t="inlineStr">
         <is>
           <t>8</t>
         </is>
       </c>
-      <c r="O10" t="inlineStr">
+      <c r="R10" t="inlineStr">
         <is>
           <t>01/04/2024</t>
         </is>
       </c>
-      <c r="P10" t="inlineStr">
+      <c r="S10" t="inlineStr">
         <is>
           <t>EN2024001</t>
         </is>
       </c>
-      <c r="Q10" t="inlineStr">
+      <c r="T10" t="inlineStr">
         <is>
           <t>APR147258369</t>
         </is>
       </c>
-      <c r="R10" t="inlineStr">
+      <c r="U10" t="inlineStr">
         <is>
           <t>901234567890</t>
         </is>
       </c>
-      <c r="S10" t="inlineStr">
+      <c r="V10" t="inlineStr">
         <is>
           <t>O+</t>
         </is>
       </c>
-      <c r="T10" t="inlineStr">
+      <c r="W10" t="inlineStr">
         <is>
           <t>Paid</t>
         </is>
       </c>
-      <c r="U10" t="inlineStr"/>
-      <c r="V10" t="inlineStr"/>
-      <c r="W10" t="inlineStr">
+      <c r="X10" t="inlineStr"/>
+      <c r="Y10" t="inlineStr"/>
+      <c r="Z10" t="inlineStr">
         <is>
           <t>Marathi</t>
         </is>
@@ -1564,98 +1717,113 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
+          <t>Delhi Public School</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>CBSE</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>2024-2025</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
           <t>Myra Desai</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="F11" t="inlineStr">
         <is>
           <t>20/07/2011</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="G11" t="inlineStr">
         <is>
           <t>Female</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="H11" t="inlineStr">
         <is>
           <t>9</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="I11" t="inlineStr">
         <is>
           <t>General</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
+      <c r="J11" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr">
+      <c r="K11" t="inlineStr">
         <is>
           <t>Harsh Desai</t>
         </is>
       </c>
-      <c r="I11" t="inlineStr">
+      <c r="L11" t="inlineStr">
         <is>
           <t>9876543228</t>
         </is>
       </c>
-      <c r="J11" t="inlineStr">
+      <c r="M11" t="inlineStr">
         <is>
           <t>Ritu Desai</t>
         </is>
       </c>
-      <c r="K11" t="inlineStr">
+      <c r="N11" t="inlineStr">
         <is>
           <t>9876543229</t>
         </is>
       </c>
-      <c r="L11" t="inlineStr">
+      <c r="O11" t="inlineStr">
         <is>
           <t>OBC</t>
         </is>
       </c>
-      <c r="M11" t="inlineStr">
+      <c r="P11" t="inlineStr">
         <is>
           <t>741 SG Highway Surat</t>
         </is>
       </c>
-      <c r="N11" t="inlineStr">
+      <c r="Q11" t="inlineStr">
         <is>
           <t>8</t>
         </is>
       </c>
-      <c r="O11" t="inlineStr">
+      <c r="R11" t="inlineStr">
         <is>
           <t>01/04/2024</t>
         </is>
       </c>
-      <c r="P11" t="inlineStr">
+      <c r="S11" t="inlineStr">
         <is>
           <t>EN2024002</t>
         </is>
       </c>
-      <c r="Q11" t="inlineStr"/>
-      <c r="R11" t="inlineStr">
+      <c r="T11" t="inlineStr"/>
+      <c r="U11" t="inlineStr">
         <is>
           <t>012345678901</t>
         </is>
       </c>
-      <c r="S11" t="inlineStr">
+      <c r="V11" t="inlineStr">
         <is>
           <t>A+</t>
         </is>
       </c>
-      <c r="T11" t="inlineStr">
+      <c r="W11" t="inlineStr">
         <is>
           <t>Pending</t>
         </is>
       </c>
-      <c r="U11" t="inlineStr"/>
-      <c r="V11" t="inlineStr"/>
-      <c r="W11" t="inlineStr">
+      <c r="X11" t="inlineStr"/>
+      <c r="Y11" t="inlineStr"/>
+      <c r="Z11" t="inlineStr">
         <is>
           <t>Gujarati</t>
         </is>
@@ -1669,102 +1837,117 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
+          <t>Modern High School</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>ICSE</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>2024-2025</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
           <t>Aadhya Iyer</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="F12" t="inlineStr">
         <is>
           <t>14/07/2009</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="G12" t="inlineStr">
         <is>
           <t>Female</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="H12" t="inlineStr">
         <is>
           <t>FYJC</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="I12" t="inlineStr">
         <is>
           <t>Science</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
+      <c r="J12" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr">
+      <c r="K12" t="inlineStr">
         <is>
           <t>Venkat Iyer</t>
         </is>
       </c>
-      <c r="I12" t="inlineStr">
+      <c r="L12" t="inlineStr">
         <is>
           <t>9876543230</t>
         </is>
       </c>
-      <c r="J12" t="inlineStr">
+      <c r="M12" t="inlineStr">
         <is>
           <t>Deepa Iyer</t>
         </is>
       </c>
-      <c r="K12" t="inlineStr">
+      <c r="N12" t="inlineStr">
         <is>
           <t>9876543231</t>
         </is>
       </c>
-      <c r="L12" t="inlineStr">
+      <c r="O12" t="inlineStr">
         <is>
           <t>General</t>
         </is>
       </c>
-      <c r="M12" t="inlineStr">
+      <c r="P12" t="inlineStr">
         <is>
           <t>852 Residency Road Bangalore</t>
         </is>
       </c>
-      <c r="N12" t="inlineStr">
+      <c r="Q12" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
-      <c r="O12" t="inlineStr">
+      <c r="R12" t="inlineStr">
         <is>
           <t>01/06/2023</t>
         </is>
       </c>
-      <c r="P12" t="inlineStr">
+      <c r="S12" t="inlineStr">
         <is>
           <t>JC2023001</t>
         </is>
       </c>
-      <c r="Q12" t="inlineStr">
+      <c r="T12" t="inlineStr">
         <is>
           <t>APR963852741</t>
         </is>
       </c>
-      <c r="R12" t="inlineStr">
+      <c r="U12" t="inlineStr">
         <is>
           <t>123098765432</t>
         </is>
       </c>
-      <c r="S12" t="inlineStr">
+      <c r="V12" t="inlineStr">
         <is>
           <t>B+</t>
         </is>
       </c>
-      <c r="T12" t="inlineStr">
+      <c r="W12" t="inlineStr">
         <is>
           <t>Paid</t>
         </is>
       </c>
-      <c r="U12" t="inlineStr"/>
-      <c r="V12" t="inlineStr"/>
-      <c r="W12" t="inlineStr">
+      <c r="X12" t="inlineStr"/>
+      <c r="Y12" t="inlineStr"/>
+      <c r="Z12" t="inlineStr">
         <is>
           <t>Kannada</t>
         </is>
@@ -1778,102 +1961,117 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
+          <t>Modern High School</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>ICSE</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>2024-2025</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
           <t>Vivaan Mehta</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="F13" t="inlineStr">
         <is>
           <t>28/02/2009</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="G13" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="H13" t="inlineStr">
         <is>
           <t>FYJC</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr">
+      <c r="I13" t="inlineStr">
         <is>
           <t>Commerce</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr">
+      <c r="J13" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="H13" t="inlineStr">
+      <c r="K13" t="inlineStr">
         <is>
           <t>Nikhil Mehta</t>
         </is>
       </c>
-      <c r="I13" t="inlineStr">
+      <c r="L13" t="inlineStr">
         <is>
           <t>9876543232</t>
         </is>
       </c>
-      <c r="J13" t="inlineStr">
+      <c r="M13" t="inlineStr">
         <is>
           <t>Sonal Mehta</t>
         </is>
       </c>
-      <c r="K13" t="inlineStr">
+      <c r="N13" t="inlineStr">
         <is>
           <t>9876543233</t>
         </is>
       </c>
-      <c r="L13" t="inlineStr">
+      <c r="O13" t="inlineStr">
         <is>
           <t>General</t>
         </is>
       </c>
-      <c r="M13" t="inlineStr">
+      <c r="P13" t="inlineStr">
         <is>
           <t>963 Linking Road Mumbai</t>
         </is>
       </c>
-      <c r="N13" t="inlineStr">
+      <c r="Q13" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
-      <c r="O13" t="inlineStr">
+      <c r="R13" t="inlineStr">
         <is>
           <t>01/06/2023</t>
         </is>
       </c>
-      <c r="P13" t="inlineStr">
+      <c r="S13" t="inlineStr">
         <is>
           <t>JC2023002</t>
         </is>
       </c>
-      <c r="Q13" t="inlineStr">
+      <c r="T13" t="inlineStr">
         <is>
           <t>APR852741963</t>
         </is>
       </c>
-      <c r="R13" t="inlineStr">
+      <c r="U13" t="inlineStr">
         <is>
           <t>234109876543</t>
         </is>
       </c>
-      <c r="S13" t="inlineStr">
+      <c r="V13" t="inlineStr">
         <is>
           <t>O+</t>
         </is>
       </c>
-      <c r="T13" t="inlineStr">
+      <c r="W13" t="inlineStr">
         <is>
           <t>Paid</t>
         </is>
       </c>
-      <c r="U13" t="inlineStr"/>
-      <c r="V13" t="inlineStr"/>
-      <c r="W13" t="inlineStr">
+      <c r="X13" t="inlineStr"/>
+      <c r="Y13" t="inlineStr"/>
+      <c r="Z13" t="inlineStr">
         <is>
           <t>English</t>
         </is>
@@ -1887,98 +2085,113 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
+          <t>Ryan International High School</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>CBSE</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>2024-2025</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
           <t>Saanvi Gupta</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="F14" t="inlineStr">
         <is>
           <t>19/05/2012</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="G14" t="inlineStr">
         <is>
           <t>Female</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
+      <c r="H14" t="inlineStr">
         <is>
           <t>8</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
+      <c r="I14" t="inlineStr">
         <is>
           <t>General</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr">
+      <c r="J14" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="H14" t="inlineStr">
+      <c r="K14" t="inlineStr">
         <is>
           <t>Rajat Gupta</t>
         </is>
       </c>
-      <c r="I14" t="inlineStr">
+      <c r="L14" t="inlineStr">
         <is>
           <t>9876543234</t>
         </is>
       </c>
-      <c r="J14" t="inlineStr">
+      <c r="M14" t="inlineStr">
         <is>
           <t>Pooja Gupta</t>
         </is>
       </c>
-      <c r="K14" t="inlineStr">
+      <c r="N14" t="inlineStr">
         <is>
           <t>9876543235</t>
         </is>
       </c>
-      <c r="L14" t="inlineStr">
+      <c r="O14" t="inlineStr">
         <is>
           <t>General</t>
         </is>
       </c>
-      <c r="M14" t="inlineStr">
+      <c r="P14" t="inlineStr">
         <is>
           <t>159 Civil Lines Jaipur</t>
         </is>
       </c>
-      <c r="N14" t="inlineStr">
+      <c r="Q14" t="inlineStr">
         <is>
           <t>7</t>
         </is>
       </c>
-      <c r="O14" t="inlineStr">
+      <c r="R14" t="inlineStr">
         <is>
           <t>01/04/2024</t>
         </is>
       </c>
-      <c r="P14" t="inlineStr">
+      <c r="S14" t="inlineStr">
         <is>
           <t>EN2024003</t>
         </is>
       </c>
-      <c r="Q14" t="inlineStr"/>
-      <c r="R14" t="inlineStr">
+      <c r="T14" t="inlineStr"/>
+      <c r="U14" t="inlineStr">
         <is>
           <t>345210987654</t>
         </is>
       </c>
-      <c r="S14" t="inlineStr">
+      <c r="V14" t="inlineStr">
         <is>
           <t>A-</t>
         </is>
       </c>
-      <c r="T14" t="inlineStr">
+      <c r="W14" t="inlineStr">
         <is>
           <t>Paid</t>
         </is>
       </c>
-      <c r="U14" t="inlineStr"/>
-      <c r="V14" t="inlineStr"/>
-      <c r="W14" t="inlineStr">
+      <c r="X14" t="inlineStr"/>
+      <c r="Y14" t="inlineStr"/>
+      <c r="Z14" t="inlineStr">
         <is>
           <t>Hindi</t>
         </is>
@@ -1992,102 +2205,117 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
+          <t>Cambridge High School</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>ICSE</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>2024-2025</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
           <t>Reyansh Verma</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="F15" t="inlineStr">
         <is>
           <t>03/10/2012</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="G15" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="H15" t="inlineStr">
         <is>
           <t>8</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="I15" t="inlineStr">
         <is>
           <t>General</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
+      <c r="J15" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="H15" t="inlineStr">
+      <c r="K15" t="inlineStr">
         <is>
           <t>Manoj Verma</t>
         </is>
       </c>
-      <c r="I15" t="inlineStr">
+      <c r="L15" t="inlineStr">
         <is>
           <t>9876543236</t>
         </is>
       </c>
-      <c r="J15" t="inlineStr">
+      <c r="M15" t="inlineStr">
         <is>
           <t>Kavita Verma</t>
         </is>
       </c>
-      <c r="K15" t="inlineStr">
+      <c r="N15" t="inlineStr">
         <is>
           <t>9876543237</t>
         </is>
       </c>
-      <c r="L15" t="inlineStr">
+      <c r="O15" t="inlineStr">
         <is>
           <t>SC</t>
         </is>
       </c>
-      <c r="M15" t="inlineStr">
+      <c r="P15" t="inlineStr">
         <is>
           <t>357 Mall Road Lucknow</t>
         </is>
       </c>
-      <c r="N15" t="inlineStr">
+      <c r="Q15" t="inlineStr">
         <is>
           <t>7</t>
         </is>
       </c>
-      <c r="O15" t="inlineStr">
+      <c r="R15" t="inlineStr">
         <is>
           <t>01/04/2024</t>
         </is>
       </c>
-      <c r="P15" t="inlineStr">
+      <c r="S15" t="inlineStr">
         <is>
           <t>EN2024004</t>
         </is>
       </c>
-      <c r="Q15" t="inlineStr">
+      <c r="T15" t="inlineStr">
         <is>
           <t>APR741852963</t>
         </is>
       </c>
-      <c r="R15" t="inlineStr">
+      <c r="U15" t="inlineStr">
         <is>
           <t>456321098765</t>
         </is>
       </c>
-      <c r="S15" t="inlineStr">
+      <c r="V15" t="inlineStr">
         <is>
           <t>B-</t>
         </is>
       </c>
-      <c r="T15" t="inlineStr">
+      <c r="W15" t="inlineStr">
         <is>
           <t>Waived</t>
         </is>
       </c>
-      <c r="U15" t="inlineStr"/>
-      <c r="V15" t="inlineStr"/>
-      <c r="W15" t="inlineStr">
+      <c r="X15" t="inlineStr"/>
+      <c r="Y15" t="inlineStr"/>
+      <c r="Z15" t="inlineStr">
         <is>
           <t>Hindi</t>
         </is>
@@ -2101,102 +2329,117 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
+          <t>St Lawrence High School</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>CBSE</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>2024-2025</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
           <t>Aanya Kapoor</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="F16" t="inlineStr">
         <is>
           <t>27/12/2010</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="G16" t="inlineStr">
         <is>
           <t>Female</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
+      <c r="H16" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr">
+      <c r="I16" t="inlineStr">
         <is>
           <t>Science</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr">
+      <c r="J16" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="H16" t="inlineStr">
+      <c r="K16" t="inlineStr">
         <is>
           <t>Ravi Kapoor</t>
         </is>
       </c>
-      <c r="I16" t="inlineStr">
+      <c r="L16" t="inlineStr">
         <is>
           <t>9876543238</t>
         </is>
       </c>
-      <c r="J16" t="inlineStr">
+      <c r="M16" t="inlineStr">
         <is>
           <t>Deepika Kapoor</t>
         </is>
       </c>
-      <c r="K16" t="inlineStr">
+      <c r="N16" t="inlineStr">
         <is>
           <t>9876543239</t>
         </is>
       </c>
-      <c r="L16" t="inlineStr">
+      <c r="O16" t="inlineStr">
         <is>
           <t>General</t>
         </is>
       </c>
-      <c r="M16" t="inlineStr">
+      <c r="P16" t="inlineStr">
         <is>
           <t>468 Sector 17 Chandigarh</t>
         </is>
       </c>
-      <c r="N16" t="inlineStr">
+      <c r="Q16" t="inlineStr">
         <is>
           <t>9</t>
         </is>
       </c>
-      <c r="O16" t="inlineStr">
+      <c r="R16" t="inlineStr">
         <is>
           <t>01/04/2023</t>
         </is>
       </c>
-      <c r="P16" t="inlineStr">
+      <c r="S16" t="inlineStr">
         <is>
           <t>EN2023005</t>
         </is>
       </c>
-      <c r="Q16" t="inlineStr">
+      <c r="T16" t="inlineStr">
         <is>
           <t>APR159753486</t>
         </is>
       </c>
-      <c r="R16" t="inlineStr">
+      <c r="U16" t="inlineStr">
         <is>
           <t>567432109876</t>
         </is>
       </c>
-      <c r="S16" t="inlineStr">
+      <c r="V16" t="inlineStr">
         <is>
           <t>AB+</t>
         </is>
       </c>
-      <c r="T16" t="inlineStr">
+      <c r="W16" t="inlineStr">
         <is>
           <t>Paid</t>
         </is>
       </c>
-      <c r="U16" t="inlineStr"/>
-      <c r="V16" t="inlineStr"/>
-      <c r="W16" t="inlineStr">
+      <c r="X16" t="inlineStr"/>
+      <c r="Y16" t="inlineStr"/>
+      <c r="Z16" t="inlineStr">
         <is>
           <t>Punjabi</t>
         </is>

</xml_diff>